<commit_message>
$RDW Q322/1 & add to Overview - Space
</commit_message>
<xml_diff>
--- a/$RDW.xlsx
+++ b/$RDW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D98ADA6-03CE-4E2B-8A08-1B4C90AC868D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73930630-FAA3-4686-82B1-B87BDA161440}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{DCD3578D-FA8F-4742-9003-583D815C10F0}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="126">
   <si>
     <t>$RDW</t>
   </si>
@@ -146,16 +146,275 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>Q322</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>COGS</t>
+  </si>
+  <si>
+    <t>Gross Profit</t>
+  </si>
+  <si>
+    <t>SG&amp;A</t>
+  </si>
+  <si>
+    <t>Transaction Expenses</t>
+  </si>
+  <si>
+    <t>Impairment Expenses</t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>Contingent Earnout Expense</t>
+  </si>
+  <si>
+    <t>Operating Income</t>
+  </si>
+  <si>
+    <t>Interest Expense, Net</t>
+  </si>
+  <si>
+    <t>Other (Income) Expense, Net</t>
+  </si>
+  <si>
+    <t>Pretax Income</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>Net Income</t>
+  </si>
+  <si>
+    <t>EPS</t>
+  </si>
+  <si>
+    <t>Revenue Y/Y</t>
+  </si>
+  <si>
+    <t>Revenue Q/Q</t>
+  </si>
+  <si>
+    <t>Gross Margin</t>
+  </si>
+  <si>
+    <t>Operating Margin</t>
+  </si>
+  <si>
+    <t>Net Margin</t>
+  </si>
+  <si>
+    <t>Tax Rate</t>
+  </si>
+  <si>
+    <t>Q222</t>
+  </si>
+  <si>
+    <t>Q122</t>
+  </si>
+  <si>
+    <t>Q421</t>
+  </si>
+  <si>
+    <t>Q321</t>
+  </si>
+  <si>
+    <t>Q221</t>
+  </si>
+  <si>
+    <t>Q121</t>
+  </si>
+  <si>
+    <t>Q420</t>
+  </si>
+  <si>
+    <t>FY20</t>
+  </si>
+  <si>
+    <t>FY21</t>
+  </si>
+  <si>
+    <t>FY22</t>
+  </si>
+  <si>
+    <t>FY23</t>
+  </si>
+  <si>
+    <t>FY24</t>
+  </si>
+  <si>
+    <t>FY25</t>
+  </si>
+  <si>
+    <t>FY26</t>
+  </si>
+  <si>
+    <t>FY27</t>
+  </si>
+  <si>
+    <t>FY28</t>
+  </si>
+  <si>
+    <t>FY29</t>
+  </si>
+  <si>
+    <t>FY30</t>
+  </si>
+  <si>
+    <t>FY31</t>
+  </si>
+  <si>
+    <t>FY32</t>
+  </si>
+  <si>
+    <t>FY33</t>
+  </si>
+  <si>
+    <t>FY34</t>
+  </si>
+  <si>
+    <t>FY35</t>
+  </si>
+  <si>
+    <t>Balance Sheet</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>Contract Assets</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>Tax Receivables</t>
+  </si>
+  <si>
+    <t>Prepaid Insurance</t>
+  </si>
+  <si>
+    <t>Prepaid Expenses &amp; OCA</t>
+  </si>
+  <si>
+    <t>TCA</t>
+  </si>
+  <si>
+    <t>PP&amp;E</t>
+  </si>
+  <si>
+    <t>ROU</t>
+  </si>
+  <si>
+    <t>Goodwill+Intangibles</t>
+  </si>
+  <si>
+    <t>Other NCA</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>Notes Payable to Sellers</t>
+  </si>
+  <si>
+    <t>Short-Term Debt</t>
+  </si>
+  <si>
+    <t>Short-Term Lease Liabilities</t>
+  </si>
+  <si>
+    <t>Accrued Expenses</t>
+  </si>
+  <si>
+    <t>Deferred Revenue</t>
+  </si>
+  <si>
+    <t>Other Current Laibilities</t>
+  </si>
+  <si>
+    <t>TCL</t>
+  </si>
+  <si>
+    <t>Long-Term Debt</t>
+  </si>
+  <si>
+    <t>Long-Term Lease Liabilities</t>
+  </si>
+  <si>
+    <t>Warrant Liabilities</t>
+  </si>
+  <si>
+    <t>Deferred Tax Liabilities</t>
+  </si>
+  <si>
+    <t>Other NCL</t>
+  </si>
+  <si>
+    <t>Liabilities</t>
+  </si>
+  <si>
+    <t>S/E</t>
+  </si>
+  <si>
+    <t>S/E+L</t>
+  </si>
+  <si>
+    <t>Book Value</t>
+  </si>
+  <si>
+    <t>Book Value per Share</t>
+  </si>
+  <si>
+    <t>Share Price</t>
+  </si>
+  <si>
+    <t>Cashflow Statement</t>
+  </si>
+  <si>
+    <t>CFFO</t>
+  </si>
+  <si>
+    <t>Acquisition of Businesses</t>
+  </si>
+  <si>
+    <t>Purchases of PP&amp;E</t>
+  </si>
+  <si>
+    <t>Purchases of Intangibles</t>
+  </si>
+  <si>
+    <t>Related Party Receivable</t>
+  </si>
+  <si>
+    <t>CFFI</t>
+  </si>
+  <si>
+    <t>CapEx</t>
+  </si>
+  <si>
+    <t>FCF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="171" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +454,31 @@
       <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Airal"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Airal"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Airal"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Airal"/>
     </font>
   </fonts>
   <fills count="6">
@@ -322,14 +606,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -364,6 +645,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -393,6 +677,47 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,6 +786,61 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{920C348A-9AA1-476B-9830-CCB4F3AABEA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6848475" y="0"/>
+          <a:ext cx="0" cy="16906875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -766,7 +1146,7 @@
   <dimension ref="A2:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:D27"/>
+      <selection activeCell="G2" sqref="G2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -795,174 +1175,192 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="G5" s="5" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="G5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="7"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>3.95</v>
       </c>
       <c r="D6" s="23"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="12"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="9">
-        <v>63.85</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="12"/>
+      <c r="C7" s="21">
+        <v>63.852690000000003</v>
+      </c>
+      <c r="D7" s="23" t="str">
+        <f>$C$28</f>
+        <v>Q322</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="21">
         <f>C6*C7</f>
-        <v>252.20750000000001</v>
+        <v>252.21812550000001</v>
       </c>
       <c r="D8" s="23"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="12"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="11"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="23"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="12"/>
+      <c r="C9" s="21">
+        <f>'Financial Model'!J67</f>
+        <v>7.0309999999999997</v>
+      </c>
+      <c r="D9" s="23" t="str">
+        <f t="shared" ref="D9:D11" si="0">$C$28</f>
+        <v>Q322</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="23"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="12"/>
+      <c r="C10" s="21">
+        <f>'Financial Model'!J68</f>
+        <v>93.988</v>
+      </c>
+      <c r="D10" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>Q322</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="11"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="21">
         <f>C9-C10</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="12"/>
+        <v>-86.956999999999994</v>
+      </c>
+      <c r="D11" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>Q322</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="11"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="22">
         <f>C8-C11</f>
-        <v>252.20750000000001</v>
+        <v>339.17512550000004</v>
       </c>
       <c r="D12" s="24"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="12"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="G13" s="19"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="12"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="11"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="G14" s="19"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="12"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="12"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
@@ -971,272 +1369,281 @@
       <c r="B16" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="12"/>
+      <c r="D16" s="15"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="11"/>
     </row>
     <row r="17" spans="2:14">
       <c r="B17" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="12"/>
+      <c r="D17" s="15"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="11"/>
     </row>
     <row r="18" spans="2:14">
       <c r="B18" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="12"/>
+      <c r="D18" s="15"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="11"/>
     </row>
     <row r="19" spans="2:14">
       <c r="B19" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="12"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="11"/>
     </row>
     <row r="20" spans="2:14">
-      <c r="G20" s="19"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="12"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="11"/>
     </row>
     <row r="21" spans="2:14">
-      <c r="G21" s="19"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="12"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="11"/>
     </row>
     <row r="22" spans="2:14">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="12"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="11"/>
     </row>
     <row r="23" spans="2:14">
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="12"/>
+      <c r="D23" s="15"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="11"/>
     </row>
     <row r="24" spans="2:14">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="14">
         <v>2020</v>
       </c>
-      <c r="D24" s="16"/>
+      <c r="D24" s="15"/>
       <c r="E24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="19"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="12"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="11"/>
     </row>
     <row r="25" spans="2:14">
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="12"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="11"/>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="19"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="16"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="12"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="11"/>
     </row>
     <row r="27" spans="2:14">
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>38</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>39</v>
       </c>
       <c r="D27" s="31"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="12"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="11"/>
     </row>
     <row r="28" spans="2:14">
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16"/>
+      <c r="C28" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="39">
+        <v>39753</v>
+      </c>
       <c r="G28" s="27">
         <v>43983</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H28" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="12"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="11"/>
     </row>
     <row r="29" spans="2:14">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="18"/>
-      <c r="G29" s="20"/>
+      <c r="C29" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="33"/>
+      <c r="G29" s="19"/>
       <c r="H29" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="14"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="13"/>
     </row>
     <row r="32" spans="2:14">
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="7"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="16"/>
+      <c r="C33" s="48">
+        <f>C6/'Financial Model'!J65</f>
+        <v>16.933667611294947</v>
+      </c>
+      <c r="D33" s="49"/>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="16"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15"/>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="16"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="15"/>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="16"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="15"/>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="16"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="15"/>
     </row>
     <row r="38" spans="2:4">
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="17"/>
-      <c r="D38" s="18"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="22">
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
@@ -1252,7 +1659,6 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B22:D22"/>
@@ -1263,34 +1669,960 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C27:D27" r:id="rId1" display="Link" xr:uid="{2A299CA7-25AE-4FFE-B4ED-AEF098FCE276}"/>
+    <hyperlink ref="C29:D29" r:id="rId2" display="Link" xr:uid="{5A3AF97E-0894-43AD-8BC8-C465C140A6E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564D0066-71C8-486E-BDC0-6D120B675537}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:AE90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="J81" sqref="J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="25.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1"/>
-    <row r="2" s="4" customFormat="1"/>
-    <row r="3" s="4" customFormat="1"/>
+    <row r="1" spans="1:31" s="34" customFormat="1">
+      <c r="C1" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="T1" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="U1" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="V1" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="W1" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="X1" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y1" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z1" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA1" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB1" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC1" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD1" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE1" s="34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="36" customFormat="1">
+      <c r="A2" s="35"/>
+      <c r="F2" s="37">
+        <v>44469</v>
+      </c>
+      <c r="J2" s="37">
+        <v>44834</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" s="36" customFormat="1">
+      <c r="A3" s="35"/>
+      <c r="J3" s="38">
+        <v>39753</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" s="45" customFormat="1">
+      <c r="B4" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="45">
+        <v>32.68</v>
+      </c>
+      <c r="J4" s="45">
+        <v>37.249000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" s="41" customFormat="1">
+      <c r="B5" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="41">
+        <v>26.786000000000001</v>
+      </c>
+      <c r="J5" s="41">
+        <v>29.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" s="45" customFormat="1">
+      <c r="B6" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="45">
+        <f t="shared" ref="C6:I6" si="0">C4-C5</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="45">
+        <f>F4-F5</f>
+        <v>5.8939999999999984</v>
+      </c>
+      <c r="G6" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="45">
+        <f>J4-J5</f>
+        <v>7.9490000000000016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" s="41" customFormat="1">
+      <c r="B7" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="41">
+        <v>34.332999999999998</v>
+      </c>
+      <c r="J7" s="41">
+        <v>15.311999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" s="41" customFormat="1">
+      <c r="B8" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="41">
+        <v>0.113</v>
+      </c>
+      <c r="J8" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" s="41" customFormat="1">
+      <c r="B9" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="41">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="J9" s="41">
+        <v>1.819</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" s="41" customFormat="1">
+      <c r="B10" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="41">
+        <v>0</v>
+      </c>
+      <c r="J10" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" s="41" customFormat="1">
+      <c r="B11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="41">
+        <v>1.371</v>
+      </c>
+      <c r="J11" s="41">
+        <v>1.133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" s="45" customFormat="1">
+      <c r="B12" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="41">
+        <f t="shared" ref="C12:I12" si="1">C6-C7-C8-C9-C10-C11</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="41">
+        <f>F6-F7-F8-F9-F10-F11</f>
+        <v>-31.050999999999998</v>
+      </c>
+      <c r="G12" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="41">
+        <f>J6-J7-J8-J9-J10-J11</f>
+        <v>-10.314999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" s="41" customFormat="1">
+      <c r="B13" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="41">
+        <v>1.74</v>
+      </c>
+      <c r="J13" s="41">
+        <v>2.4009999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" s="41" customFormat="1">
+      <c r="B14" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="41">
+        <v>-2.9569999999999999</v>
+      </c>
+      <c r="J14" s="41">
+        <v>-0.158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" s="41" customFormat="1">
+      <c r="B15" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="41">
+        <f t="shared" ref="C15:I15" si="2">C12-C13-C14</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="41">
+        <f>F12-F13-F14</f>
+        <v>-29.833999999999996</v>
+      </c>
+      <c r="G15" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="41">
+        <f>J12-J13-J14</f>
+        <v>-12.557999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" s="41" customFormat="1">
+      <c r="B16" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="41">
+        <v>-5.5819999999999999</v>
+      </c>
+      <c r="J16" s="41">
+        <v>-2.1349999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" s="45" customFormat="1">
+      <c r="B17" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="45">
+        <f t="shared" ref="C17:I17" si="3">C15-C16</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="45">
+        <f>F15-F16</f>
+        <v>-24.251999999999995</v>
+      </c>
+      <c r="G17" s="45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="45">
+        <f>J15-J16</f>
+        <v>-10.422999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" s="43" customFormat="1">
+      <c r="B18" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="43">
+        <f>F17/F19</f>
+        <v>-0.55073071965599074</v>
+      </c>
+      <c r="J18" s="43">
+        <f>J17/J19</f>
+        <v>-0.16424382986923508</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" s="41" customFormat="1">
+      <c r="B19" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="41">
+        <v>44.03604</v>
+      </c>
+      <c r="J19" s="41">
+        <v>63.460526999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" s="40" customFormat="1">
+      <c r="B21" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="44">
+        <f>J4/F4-1</f>
+        <v>0.13981028151774799</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="42">
+        <f>F6/F4</f>
+        <v>0.18035495716034267</v>
+      </c>
+      <c r="J24" s="42">
+        <f>J6/J4</f>
+        <v>0.21340170205911571</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="42">
+        <f>F12/F4</f>
+        <v>-0.95015299877600978</v>
+      </c>
+      <c r="J25" s="42">
+        <f>J12/J4</f>
+        <v>-0.27692018577679928</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="42">
+        <f>F17/F4</f>
+        <v>-0.7421052631578946</v>
+      </c>
+      <c r="J26" s="42">
+        <f>J17/J4</f>
+        <v>-0.27981959247228105</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="42">
+        <f>F16/F15</f>
+        <v>0.1871019642019173</v>
+      </c>
+      <c r="J27" s="42">
+        <f>J16/J15</f>
+        <v>0.17001114827201785</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" s="40" customFormat="1">
+      <c r="B32" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="J32" s="45">
+        <v>7.0309999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J33" s="41">
+        <v>16.521000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J34" s="41">
+        <v>16.318999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J35" s="41">
+        <v>2.0289999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J36" s="41">
+        <v>0.68799999999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J37" s="41">
+        <v>3.0459999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J38" s="41">
+        <v>3.7250000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" ref="C39:I39" si="4">SUM(C32:C38)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="41">
+        <f>SUM(J32:J38)</f>
+        <v>49.358999999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J40" s="41">
+        <v>6.6970000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J41" s="41">
+        <v>14.782999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J42" s="41">
+        <f>56.207+56.71</f>
+        <v>112.917</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="B43" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J43" s="41">
+        <v>0.61599999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="B44" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" ref="C44:I44" si="5">C39+SUM(C40:C43)</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G44" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H44" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I44" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="41">
+        <f>J39+SUM(J40:J43)</f>
+        <v>184.37200000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="J45" s="41"/>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="B46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J46" s="41">
+        <v>17.594999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" s="40" customFormat="1">
+      <c r="B47" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="J47" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" s="40" customFormat="1">
+      <c r="B48" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="J48" s="45">
+        <v>3.476</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="B49" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J49" s="41">
+        <v>3.484</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="B50" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J50" s="41">
+        <v>18.908999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="B51" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J51" s="41">
+        <v>17.373000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="B52" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J52" s="41">
+        <v>1.786</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="B53" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" ref="C53:I53" si="6">SUM(C46:C52)</f>
+        <v>0</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G53" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H53" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I53" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J53" s="41">
+        <f>SUM(J46:J52)</f>
+        <v>63.623000000000005</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" s="40" customFormat="1">
+      <c r="B54" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="J54" s="45">
+        <v>89.512</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J55" s="41">
+        <v>11.379</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J56" s="41">
+        <v>3.093</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10">
+      <c r="B57" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J57" s="41">
+        <v>1.637</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="B58" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J58" s="41">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10">
+      <c r="B59" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" s="3">
+        <f t="shared" ref="C59:I59" si="7">SUM(C53:C58)</f>
+        <v>0</v>
+      </c>
+      <c r="D59" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E59" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G59" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H59" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I59" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J59" s="41">
+        <f>SUM(J53:J58)</f>
+        <v>169.56899999999996</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10">
+      <c r="J60" s="41"/>
+    </row>
+    <row r="61" spans="2:10">
+      <c r="B61" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J61" s="41">
+        <v>14.803000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10">
+      <c r="B62" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J62" s="41">
+        <f>J61+J59</f>
+        <v>184.37199999999996</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10">
+      <c r="B64" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J64" s="41">
+        <f>J44-J59</f>
+        <v>14.803000000000054</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10">
+      <c r="B65" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J65" s="3">
+        <f>J64/J19</f>
+        <v>0.23326311172928102</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10">
+      <c r="B67" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J67" s="41">
+        <f>J32</f>
+        <v>7.0309999999999997</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10">
+      <c r="B68" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J68" s="41">
+        <f>J47+J48+J54</f>
+        <v>93.988</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10">
+      <c r="B69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J69" s="41">
+        <f>J67-J68</f>
+        <v>-86.956999999999994</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10">
+      <c r="B71" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J71" s="3">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10">
+      <c r="B72" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J72" s="41">
+        <f>J71*J19</f>
+        <v>151.03605425999999</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10">
+      <c r="B73" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J73" s="41">
+        <f>J72-J69</f>
+        <v>237.99305425999998</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10">
+      <c r="B75" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J75" s="50">
+        <f>J71/J65</f>
+        <v>10.203070611362524</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10">
+      <c r="B79" s="47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" s="40" customFormat="1">
+      <c r="B87" s="40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" s="40" customFormat="1">
+      <c r="B90" s="40" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J1" r:id="rId1" location="ieb75bb50d25b43988f02e27af34ce5ea_19" xr:uid="{F3BAE21F-8075-4AD3-AE46-BE3F41688B15}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
$RDW Q1 & Q2 21/2
</commit_message>
<xml_diff>
--- a/$RDW.xlsx
+++ b/$RDW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73930630-FAA3-4686-82B1-B87BDA161440}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3B26E6-D15A-4430-A498-649976A94BCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{DCD3578D-FA8F-4742-9003-583D815C10F0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{DCD3578D-FA8F-4742-9003-583D815C10F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="171" formatCode="0.0\x"/>
+    <numFmt numFmtId="165" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -611,15 +611,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -627,18 +618,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -668,21 +647,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -711,13 +675,49 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1145,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDBB179-D49E-4949-9A72-224211CC16A1}">
   <dimension ref="A2:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:N2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1158,16 +1158,16 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
     </row>
     <row r="3" spans="1:14">
       <c r="B3" s="2" t="s">
@@ -1175,475 +1175,481 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="G5" s="4" t="s">
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="G5" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="6"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="46"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="5">
         <v>3.95</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="11"/>
+      <c r="D6" s="16"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="14">
         <v>63.852690000000003</v>
       </c>
-      <c r="D7" s="23" t="str">
+      <c r="D7" s="16" t="str">
         <f>$C$28</f>
         <v>Q322</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="8"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="14">
         <f>C6*C7</f>
         <v>252.21812550000001</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="11"/>
+      <c r="D8" s="16"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="14">
         <f>'Financial Model'!J67</f>
         <v>7.0309999999999997</v>
       </c>
-      <c r="D9" s="23" t="str">
+      <c r="D9" s="16" t="str">
         <f t="shared" ref="D9:D11" si="0">$C$28</f>
         <v>Q322</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="14">
         <f>'Financial Model'!J68</f>
         <v>93.988</v>
       </c>
-      <c r="D10" s="23" t="str">
+      <c r="D10" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Q322</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="14">
         <f>C9-C10</f>
         <v>-86.956999999999994</v>
       </c>
-      <c r="D11" s="23" t="str">
+      <c r="D11" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Q322</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="8"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="15">
         <f>C8-C11</f>
         <v>339.17512550000004</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="11"/>
+      <c r="D12" s="17"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="8"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="G13" s="18"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="G14" s="18"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="8"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="11"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="46"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="8"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="11"/>
+      <c r="D16" s="38"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="8"/>
     </row>
     <row r="17" spans="2:14">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="11"/>
+      <c r="D17" s="38"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="8"/>
     </row>
     <row r="18" spans="2:14">
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="11"/>
+      <c r="D18" s="38"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="8"/>
     </row>
     <row r="19" spans="2:14">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="17"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="11"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="8"/>
     </row>
     <row r="20" spans="2:14">
-      <c r="G20" s="18"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="8"/>
     </row>
     <row r="21" spans="2:14">
-      <c r="G21" s="18"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="8"/>
     </row>
     <row r="22" spans="2:14">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="11"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="46"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="8"/>
     </row>
     <row r="23" spans="2:14">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="11"/>
+      <c r="D23" s="38"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="8"/>
     </row>
     <row r="24" spans="2:14">
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="37">
         <v>2020</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="8"/>
     </row>
     <row r="25" spans="2:14">
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="15"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="11"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="38"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="8"/>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="18"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="15"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="38"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="8"/>
     </row>
     <row r="27" spans="2:14">
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="31"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="11"/>
+      <c r="D27" s="50"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="8"/>
     </row>
     <row r="28" spans="2:14">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="39">
+      <c r="D28" s="27">
         <v>39753</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G28" s="20">
         <v>43983</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="H28" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="11"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="8"/>
     </row>
     <row r="29" spans="2:14">
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="28" t="s">
+      <c r="D29" s="43"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="13"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="10"/>
     </row>
     <row r="32" spans="2:14">
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="46"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="48">
+      <c r="C33" s="47">
         <f>C6/'Financial Model'!J65</f>
         <v>16.933667611294947</v>
       </c>
-      <c r="D33" s="49"/>
+      <c r="D33" s="48"/>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="15"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="38"/>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="38"/>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="15"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="38"/>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="15"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="38"/>
     </row>
     <row r="38" spans="2:4">
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="17"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
@@ -1660,12 +1666,6 @@
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C27:D27" r:id="rId1" display="Link" xr:uid="{2A299CA7-25AE-4FFE-B4ED-AEF098FCE276}"/>
@@ -1681,11 +1681,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564D0066-71C8-486E-BDC0-6D120B675537}">
   <dimension ref="A1:AE90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J81" sqref="J81"/>
+      <selection pane="bottomRight" activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1695,20 +1695,20 @@
     <col min="3" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="34" customFormat="1">
-      <c r="C1" s="34" t="s">
+    <row r="1" spans="1:31" s="22" customFormat="1">
+      <c r="C1" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="22" t="s">
         <v>64</v>
       </c>
       <c r="H1" s="34" t="s">
@@ -1717,431 +1717,693 @@
       <c r="I1" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="R1" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="S1" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="T1" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="U1" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="V1" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="W1" s="34" t="s">
+      <c r="W1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="X1" s="34" t="s">
+      <c r="X1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="Y1" s="34" t="s">
+      <c r="Y1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="Z1" s="34" t="s">
+      <c r="Z1" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="AA1" s="34" t="s">
+      <c r="AA1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="AB1" s="34" t="s">
+      <c r="AB1" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AC1" s="34" t="s">
+      <c r="AC1" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="AD1" s="34" t="s">
+      <c r="AD1" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="AE1" s="34" t="s">
+      <c r="AE1" s="22" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="36" customFormat="1">
-      <c r="A2" s="35"/>
-      <c r="F2" s="37">
+    <row r="2" spans="1:31" s="24" customFormat="1">
+      <c r="A2" s="23"/>
+      <c r="D2" s="25">
+        <v>44286</v>
+      </c>
+      <c r="E2" s="25">
+        <v>44377</v>
+      </c>
+      <c r="F2" s="25">
         <v>44469</v>
       </c>
-      <c r="J2" s="37">
+      <c r="H2" s="25">
+        <v>44651</v>
+      </c>
+      <c r="I2" s="25">
+        <v>44742</v>
+      </c>
+      <c r="J2" s="25">
         <v>44834</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="36" customFormat="1">
-      <c r="A3" s="35"/>
-      <c r="J3" s="38">
+    <row r="3" spans="1:31" s="24" customFormat="1">
+      <c r="A3" s="23"/>
+      <c r="H3" s="26">
+        <v>41030</v>
+      </c>
+      <c r="I3" s="26">
+        <v>40391</v>
+      </c>
+      <c r="J3" s="26">
         <v>39753</v>
       </c>
     </row>
-    <row r="4" spans="1:31" s="45" customFormat="1">
-      <c r="B4" s="45" t="s">
+    <row r="4" spans="1:31" s="33" customFormat="1">
+      <c r="B4" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="45">
+      <c r="D4" s="33">
+        <v>31.698</v>
+      </c>
+      <c r="E4" s="33">
+        <v>32.148000000000003</v>
+      </c>
+      <c r="F4" s="33">
         <v>32.68</v>
       </c>
-      <c r="J4" s="45">
+      <c r="H4" s="33">
+        <v>32.866999999999997</v>
+      </c>
+      <c r="I4" s="33">
+        <v>36.728000000000002</v>
+      </c>
+      <c r="J4" s="33">
         <v>37.249000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:31" s="41" customFormat="1">
-      <c r="B5" s="41" t="s">
+    <row r="5" spans="1:31" s="29" customFormat="1">
+      <c r="B5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="41">
+      <c r="D5" s="29">
+        <v>24.221</v>
+      </c>
+      <c r="E5" s="29">
+        <v>23.533999999999999</v>
+      </c>
+      <c r="F5" s="29">
         <v>26.786000000000001</v>
       </c>
-      <c r="J5" s="41">
+      <c r="H5" s="29">
+        <v>27.696000000000002</v>
+      </c>
+      <c r="I5" s="29">
+        <v>29.745999999999999</v>
+      </c>
+      <c r="J5" s="29">
         <v>29.3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" s="45" customFormat="1">
-      <c r="B6" s="45" t="s">
+    <row r="6" spans="1:31" s="33" customFormat="1">
+      <c r="B6" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="33">
         <f t="shared" ref="C6:I6" si="0">C4-C5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="45">
+        <v>7.4770000000000003</v>
+      </c>
+      <c r="E6" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="45">
+        <v>8.6140000000000043</v>
+      </c>
+      <c r="F6" s="33">
         <f>F4-F5</f>
         <v>5.8939999999999984</v>
       </c>
-      <c r="G6" s="45">
+      <c r="G6" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="45">
+      <c r="H6" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="45">
+        <v>5.1709999999999958</v>
+      </c>
+      <c r="I6" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="45">
+        <v>6.9820000000000029</v>
+      </c>
+      <c r="J6" s="33">
         <f>J4-J5</f>
         <v>7.9490000000000016</v>
       </c>
     </row>
-    <row r="7" spans="1:31" s="41" customFormat="1">
-      <c r="B7" s="41" t="s">
+    <row r="7" spans="1:31" s="29" customFormat="1">
+      <c r="B7" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="41">
+      <c r="D7" s="29">
+        <v>11.256</v>
+      </c>
+      <c r="E7" s="29">
+        <v>12.143000000000001</v>
+      </c>
+      <c r="F7" s="29">
         <v>34.332999999999998</v>
       </c>
-      <c r="J7" s="41">
+      <c r="H7" s="29">
+        <v>20.951000000000001</v>
+      </c>
+      <c r="I7" s="29">
+        <v>17.562000000000001</v>
+      </c>
+      <c r="J7" s="29">
         <v>15.311999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:31" s="41" customFormat="1">
-      <c r="B8" s="41" t="s">
+    <row r="8" spans="1:31" s="29" customFormat="1">
+      <c r="B8" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="41">
+      <c r="D8" s="29">
+        <v>0</v>
+      </c>
+      <c r="E8" s="29">
+        <v>11.114000000000001</v>
+      </c>
+      <c r="F8" s="29">
         <v>0.113</v>
       </c>
-      <c r="J8" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" s="41" customFormat="1">
-      <c r="B9" s="41" t="s">
+      <c r="H8" s="29">
+        <v>0</v>
+      </c>
+      <c r="I8" s="29">
+        <v>0</v>
+      </c>
+      <c r="J8" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" s="29" customFormat="1">
+      <c r="B9" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="41">
+      <c r="D9" s="29">
+        <v>2.4169999999999998</v>
+      </c>
+      <c r="E9" s="29">
+        <v>2E-3</v>
+      </c>
+      <c r="F9" s="29">
         <v>1.1279999999999999</v>
       </c>
-      <c r="J9" s="41">
+      <c r="H9" s="29">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="I9" s="29">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="J9" s="29">
         <v>1.819</v>
       </c>
     </row>
-    <row r="10" spans="1:31" s="41" customFormat="1">
-      <c r="B10" s="41" t="s">
+    <row r="10" spans="1:31" s="29" customFormat="1">
+      <c r="B10" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="41">
-        <v>0</v>
-      </c>
-      <c r="J10" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" s="41" customFormat="1">
-      <c r="B11" s="41" t="s">
+      <c r="D10" s="29">
+        <v>0</v>
+      </c>
+      <c r="E10" s="29">
+        <v>0</v>
+      </c>
+      <c r="F10" s="29">
+        <v>0</v>
+      </c>
+      <c r="H10" s="29">
+        <v>0</v>
+      </c>
+      <c r="I10" s="29">
+        <v>80.462000000000003</v>
+      </c>
+      <c r="J10" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" s="29" customFormat="1">
+      <c r="B11" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="41">
+      <c r="D11" s="29">
+        <v>0.996</v>
+      </c>
+      <c r="E11" s="29">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="F11" s="29">
         <v>1.371</v>
       </c>
-      <c r="J11" s="41">
+      <c r="H11" s="29">
+        <v>1.724</v>
+      </c>
+      <c r="I11" s="29">
+        <v>1.708</v>
+      </c>
+      <c r="J11" s="29">
         <v>1.133</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="45" customFormat="1">
-      <c r="B12" s="45" t="s">
+    <row r="12" spans="1:31" s="33" customFormat="1">
+      <c r="B12" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="29">
         <f t="shared" ref="C12:I12" si="1">C6-C7-C8-C9-C10-C11</f>
         <v>0</v>
       </c>
-      <c r="D12" s="41">
+      <c r="D12" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="41">
+        <v>-7.1920000000000002</v>
+      </c>
+      <c r="E12" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="41">
+        <v>-15.602999999999998</v>
+      </c>
+      <c r="F12" s="29">
         <f>F6-F7-F8-F9-F10-F11</f>
         <v>-31.050999999999998</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H12" s="41">
+      <c r="H12" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="41">
+        <v>-17.550000000000004</v>
+      </c>
+      <c r="I12" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="41">
+        <v>-92.798000000000002</v>
+      </c>
+      <c r="J12" s="29">
         <f>J6-J7-J8-J9-J10-J11</f>
         <v>-10.314999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:31" s="41" customFormat="1">
-      <c r="B13" s="41" t="s">
+    <row r="13" spans="1:31" s="29" customFormat="1">
+      <c r="B13" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="41">
+      <c r="D13" s="29">
+        <v>1.421</v>
+      </c>
+      <c r="E13" s="29">
+        <v>1.77</v>
+      </c>
+      <c r="F13" s="29">
         <v>1.74</v>
       </c>
-      <c r="J13" s="41">
+      <c r="H13" s="29">
+        <v>1.452</v>
+      </c>
+      <c r="I13" s="29">
+        <v>1.67</v>
+      </c>
+      <c r="J13" s="29">
         <v>2.4009999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:31" s="41" customFormat="1">
-      <c r="B14" s="41" t="s">
+    <row r="14" spans="1:31" s="29" customFormat="1">
+      <c r="B14" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="41">
+      <c r="D14" s="29">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="E14" s="29">
+        <v>-0.11</v>
+      </c>
+      <c r="F14" s="29">
         <v>-2.9569999999999999</v>
       </c>
-      <c r="J14" s="41">
+      <c r="H14" s="29">
+        <v>1.18</v>
+      </c>
+      <c r="I14" s="29">
+        <v>-15.515000000000001</v>
+      </c>
+      <c r="J14" s="29">
         <v>-0.158</v>
       </c>
     </row>
-    <row r="15" spans="1:31" s="41" customFormat="1">
-      <c r="B15" s="41" t="s">
+    <row r="15" spans="1:31" s="29" customFormat="1">
+      <c r="B15" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="41">
+      <c r="C15" s="29">
         <f t="shared" ref="C15:I15" si="2">C12-C13-C14</f>
         <v>0</v>
       </c>
-      <c r="D15" s="41">
+      <c r="D15" s="29">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="41">
+        <v>-8.6999999999999993</v>
+      </c>
+      <c r="E15" s="29">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="41">
+        <v>-17.262999999999998</v>
+      </c>
+      <c r="F15" s="29">
         <f>F12-F13-F14</f>
         <v>-29.833999999999996</v>
       </c>
-      <c r="G15" s="41">
+      <c r="G15" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H15" s="41">
+      <c r="H15" s="29">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="41">
+        <v>-20.182000000000002</v>
+      </c>
+      <c r="I15" s="29">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="41">
+        <v>-78.953000000000003</v>
+      </c>
+      <c r="J15" s="29">
         <f>J12-J13-J14</f>
         <v>-12.557999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:31" s="41" customFormat="1">
-      <c r="B16" s="41" t="s">
+    <row r="16" spans="1:31" s="29" customFormat="1">
+      <c r="B16" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="41">
+      <c r="D16" s="29">
+        <v>-1.026</v>
+      </c>
+      <c r="E16" s="29">
+        <v>-1.3620000000000001</v>
+      </c>
+      <c r="F16" s="29">
         <v>-5.5819999999999999</v>
       </c>
-      <c r="J16" s="41">
+      <c r="H16" s="29">
+        <v>-2.8889999999999998</v>
+      </c>
+      <c r="I16" s="29">
+        <v>-1.925</v>
+      </c>
+      <c r="J16" s="29">
         <v>-2.1349999999999998</v>
       </c>
     </row>
-    <row r="17" spans="2:10" s="45" customFormat="1">
-      <c r="B17" s="45" t="s">
+    <row r="17" spans="2:11" s="33" customFormat="1">
+      <c r="B17" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="33">
         <f t="shared" ref="C17:I17" si="3">C15-C16</f>
         <v>0</v>
       </c>
-      <c r="D17" s="45">
+      <c r="D17" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="45">
+        <v>-7.6739999999999995</v>
+      </c>
+      <c r="E17" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="45">
+        <v>-15.900999999999998</v>
+      </c>
+      <c r="F17" s="33">
         <f>F15-F16</f>
         <v>-24.251999999999995</v>
       </c>
-      <c r="G17" s="45">
+      <c r="G17" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H17" s="45">
+      <c r="H17" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="45">
+        <v>-17.293000000000003</v>
+      </c>
+      <c r="I17" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="45">
+        <v>-77.028000000000006</v>
+      </c>
+      <c r="J17" s="33">
         <f>J15-J16</f>
         <v>-10.422999999999998</v>
       </c>
     </row>
-    <row r="18" spans="2:10" s="43" customFormat="1">
-      <c r="B18" s="43" t="s">
+    <row r="18" spans="2:11" s="31" customFormat="1">
+      <c r="B18" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="43">
+      <c r="D18" s="31">
+        <f>D17/D19</f>
+        <v>-0.20629032258064514</v>
+      </c>
+      <c r="E18" s="31">
+        <f>E17/E19</f>
+        <v>-0.42744623655913971</v>
+      </c>
+      <c r="F18" s="31">
         <f>F17/F19</f>
         <v>-0.55073071965599074</v>
       </c>
-      <c r="J18" s="43">
+      <c r="H18" s="31">
+        <f>H17/H19</f>
+        <v>-0.27584559403698811</v>
+      </c>
+      <c r="I18" s="31">
+        <f>I17/I19</f>
+        <v>-1.2228131325063158</v>
+      </c>
+      <c r="J18" s="31">
         <f>J17/J19</f>
         <v>-0.16424382986923508</v>
       </c>
     </row>
-    <row r="19" spans="2:10" s="41" customFormat="1">
-      <c r="B19" s="41" t="s">
+    <row r="19" spans="2:11" s="29" customFormat="1">
+      <c r="B19" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="41">
+      <c r="D19" s="29">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E19" s="29">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="F19" s="29">
         <v>44.03604</v>
       </c>
-      <c r="J19" s="41">
+      <c r="H19" s="29">
+        <v>62.690868999999999</v>
+      </c>
+      <c r="I19" s="29">
+        <v>62.992454000000002</v>
+      </c>
+      <c r="J19" s="29">
         <v>63.460526999999999</v>
       </c>
     </row>
-    <row r="21" spans="2:10" s="40" customFormat="1">
-      <c r="B21" s="40" t="s">
+    <row r="21" spans="2:11" s="28" customFormat="1">
+      <c r="B21" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="44">
+      <c r="F21" s="30"/>
+      <c r="H21" s="32">
+        <f>H4/D4-1</f>
+        <v>3.6879298378446501E-2</v>
+      </c>
+      <c r="I21" s="32">
+        <f>I4/E4-1</f>
+        <v>0.14246609431379853</v>
+      </c>
+      <c r="J21" s="32">
         <f>J4/F4-1</f>
         <v>0.13981028151774799</v>
       </c>
-    </row>
-    <row r="22" spans="2:10">
+      <c r="K21" s="32"/>
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="2:10">
+      <c r="E22" s="30">
+        <f>E4/D4-1</f>
+        <v>1.4196479273140383E-2</v>
+      </c>
+      <c r="F22" s="30">
+        <f>F4/E4-1</f>
+        <v>1.6548463356973908E-2</v>
+      </c>
+      <c r="I22" s="30">
+        <f>I4/H4-1</f>
+        <v>0.1174734536160893</v>
+      </c>
+      <c r="J22" s="30">
+        <f>J4/I4-1</f>
+        <v>1.4185362666085943E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
       <c r="B24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="42">
+      <c r="D24" s="30">
+        <f t="shared" ref="D24:E24" si="4">D6/D4</f>
+        <v>0.23588239005615497</v>
+      </c>
+      <c r="E24" s="30">
+        <f t="shared" ref="E24:F24" si="5">E6/E4</f>
+        <v>0.26794823939280837</v>
+      </c>
+      <c r="F24" s="30">
         <f>F6/F4</f>
         <v>0.18035495716034267</v>
       </c>
-      <c r="J24" s="42">
+      <c r="H24" s="30">
+        <f t="shared" ref="H24:I24" si="6">H6/H4</f>
+        <v>0.15733106155109977</v>
+      </c>
+      <c r="I24" s="30">
+        <f t="shared" ref="I24:J24" si="7">I6/I4</f>
+        <v>0.19010019603572215</v>
+      </c>
+      <c r="J24" s="30">
         <f>J6/J4</f>
         <v>0.21340170205911571</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:11">
       <c r="B25" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="42">
+      <c r="D25" s="30">
+        <f t="shared" ref="D25:E25" si="8">D12/D4</f>
+        <v>-0.22689128651649948</v>
+      </c>
+      <c r="E25" s="30">
+        <f t="shared" ref="E25:F25" si="9">E12/E4</f>
+        <v>-0.48534901082493459</v>
+      </c>
+      <c r="F25" s="30">
         <f>F12/F4</f>
         <v>-0.95015299877600978</v>
       </c>
-      <c r="J25" s="42">
+      <c r="H25" s="30">
+        <f t="shared" ref="H25:I25" si="10">H12/H4</f>
+        <v>-0.53397024370949597</v>
+      </c>
+      <c r="I25" s="30">
+        <f t="shared" ref="I25:J25" si="11">I12/I4</f>
+        <v>-2.5266281855804835</v>
+      </c>
+      <c r="J25" s="30">
         <f>J12/J4</f>
         <v>-0.27692018577679928</v>
       </c>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" spans="2:11">
       <c r="B26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="42">
+      <c r="D26" s="30">
+        <f t="shared" ref="D26:E26" si="12">D17/D4</f>
+        <v>-0.24209729320461856</v>
+      </c>
+      <c r="E26" s="30">
+        <f t="shared" ref="E26:F26" si="13">E17/E4</f>
+        <v>-0.49461863879557039</v>
+      </c>
+      <c r="F26" s="30">
         <f>F17/F4</f>
         <v>-0.7421052631578946</v>
       </c>
-      <c r="J26" s="42">
+      <c r="H26" s="30">
+        <f t="shared" ref="H26:I26" si="14">H17/H4</f>
+        <v>-0.52615085039705489</v>
+      </c>
+      <c r="I26" s="30">
+        <f t="shared" ref="I26:J26" si="15">I17/I4</f>
+        <v>-2.0972554998910913</v>
+      </c>
+      <c r="J26" s="30">
         <f>J17/J4</f>
         <v>-0.27981959247228105</v>
       </c>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="2:11">
       <c r="B27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="42">
+      <c r="D27" s="30">
+        <f t="shared" ref="D27:E27" si="16">D16/D15</f>
+        <v>0.11793103448275863</v>
+      </c>
+      <c r="E27" s="30">
+        <f t="shared" ref="E27:F27" si="17">E16/E15</f>
+        <v>7.889706308289407E-2</v>
+      </c>
+      <c r="F27" s="30">
         <f>F16/F15</f>
         <v>0.1871019642019173</v>
       </c>
-      <c r="J27" s="42">
+      <c r="H27" s="30">
+        <f t="shared" ref="H27:I27" si="18">H16/H15</f>
+        <v>0.14314735903280149</v>
+      </c>
+      <c r="I27" s="30">
+        <f t="shared" ref="I27:J27" si="19">I16/I15</f>
+        <v>2.4381594112953275E-2</v>
+      </c>
+      <c r="J27" s="30">
         <f>J16/J15</f>
         <v>0.17001114827201785</v>
       </c>
     </row>
-    <row r="31" spans="2:10">
-      <c r="B31" s="47" t="s">
+    <row r="31" spans="2:11">
+      <c r="B31" s="35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="2:10" s="40" customFormat="1">
-      <c r="B32" s="40" t="s">
+    <row r="32" spans="2:11" s="28" customFormat="1">
+      <c r="B32" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="J32" s="45">
+      <c r="H32" s="33">
+        <v>5.9379999999999997</v>
+      </c>
+      <c r="I32" s="33">
+        <v>10.879</v>
+      </c>
+      <c r="J32" s="33">
         <v>7.0309999999999997</v>
       </c>
     </row>
@@ -2149,7 +2411,13 @@
       <c r="B33" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="J33" s="41">
+      <c r="H33" s="29">
+        <v>11.984</v>
+      </c>
+      <c r="I33" s="29">
+        <v>12.702</v>
+      </c>
+      <c r="J33" s="29">
         <v>16.521000000000001</v>
       </c>
     </row>
@@ -2157,7 +2425,13 @@
       <c r="B34" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J34" s="41">
+      <c r="H34" s="29">
+        <v>17.492000000000001</v>
+      </c>
+      <c r="I34" s="29">
+        <v>14.747</v>
+      </c>
+      <c r="J34" s="29">
         <v>16.318999999999999</v>
       </c>
     </row>
@@ -2165,7 +2439,13 @@
       <c r="B35" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J35" s="41">
+      <c r="H35" s="29">
+        <v>1.022</v>
+      </c>
+      <c r="I35" s="29">
+        <v>1.681</v>
+      </c>
+      <c r="J35" s="29">
         <v>2.0289999999999999</v>
       </c>
     </row>
@@ -2173,7 +2453,13 @@
       <c r="B36" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J36" s="41">
+      <c r="H36" s="29">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="I36" s="29">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="J36" s="29">
         <v>0.68799999999999994</v>
       </c>
     </row>
@@ -2181,7 +2467,13 @@
       <c r="B37" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J37" s="41">
+      <c r="H37" s="29">
+        <v>1.752</v>
+      </c>
+      <c r="I37" s="29">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="J37" s="29">
         <v>3.0459999999999998</v>
       </c>
     </row>
@@ -2189,7 +2481,13 @@
       <c r="B38" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J38" s="41">
+      <c r="H38" s="29">
+        <v>4.593</v>
+      </c>
+      <c r="I38" s="29">
+        <v>4.0730000000000004</v>
+      </c>
+      <c r="J38" s="29">
         <v>3.7250000000000001</v>
       </c>
     </row>
@@ -2198,34 +2496,34 @@
         <v>92</v>
       </c>
       <c r="C39" s="3">
-        <f t="shared" ref="C39:I39" si="4">SUM(C32:C38)</f>
+        <f t="shared" ref="C39:I39" si="20">SUM(C32:C38)</f>
         <v>0</v>
       </c>
       <c r="D39" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="E39" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="G39" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H39" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I39" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J39" s="41">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="29">
+        <f t="shared" si="20"/>
+        <v>43.469000000000008</v>
+      </c>
+      <c r="I39" s="29">
+        <f t="shared" si="20"/>
+        <v>45.442</v>
+      </c>
+      <c r="J39" s="29">
         <f>SUM(J32:J38)</f>
         <v>49.358999999999995</v>
       </c>
@@ -2234,7 +2532,13 @@
       <c r="B40" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="J40" s="41">
+      <c r="H40" s="29">
+        <v>18.786000000000001</v>
+      </c>
+      <c r="I40" s="29">
+        <v>5.8239999999999998</v>
+      </c>
+      <c r="J40" s="29">
         <v>6.6970000000000001</v>
       </c>
     </row>
@@ -2242,7 +2546,13 @@
       <c r="B41" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="J41" s="41">
+      <c r="H41" s="29">
+        <v>12.984999999999999</v>
+      </c>
+      <c r="I41" s="29">
+        <v>12.08</v>
+      </c>
+      <c r="J41" s="29">
         <v>14.782999999999999</v>
       </c>
     </row>
@@ -2250,7 +2560,15 @@
       <c r="B42" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J42" s="41">
+      <c r="H42" s="29">
+        <f>96.23+88.352</f>
+        <v>184.58199999999999</v>
+      </c>
+      <c r="I42" s="29">
+        <f>57.724+56.752</f>
+        <v>114.476</v>
+      </c>
+      <c r="J42" s="29">
         <f>56.207+56.71</f>
         <v>112.917</v>
       </c>
@@ -2259,7 +2577,13 @@
       <c r="B43" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J43" s="41">
+      <c r="H43" s="29">
+        <v>0</v>
+      </c>
+      <c r="I43" s="29">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="J43" s="29">
         <v>0.61599999999999999</v>
       </c>
     </row>
@@ -2268,62 +2592,80 @@
         <v>97</v>
       </c>
       <c r="C44" s="3">
-        <f t="shared" ref="C44:I44" si="5">C39+SUM(C40:C43)</f>
+        <f t="shared" ref="C44:I44" si="21">C39+SUM(C40:C43)</f>
         <v>0</v>
       </c>
       <c r="D44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="E44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="F44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="G44" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H44" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I44" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J44" s="41">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="H44" s="29">
+        <f t="shared" si="21"/>
+        <v>259.822</v>
+      </c>
+      <c r="I44" s="29">
+        <f t="shared" si="21"/>
+        <v>178.578</v>
+      </c>
+      <c r="J44" s="29">
         <f>J39+SUM(J40:J43)</f>
         <v>184.37200000000001</v>
       </c>
     </row>
     <row r="45" spans="2:10">
-      <c r="J45" s="41"/>
+      <c r="J45" s="29"/>
     </row>
     <row r="46" spans="2:10">
       <c r="B46" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J46" s="41">
+      <c r="H46" s="29">
+        <v>13.904999999999999</v>
+      </c>
+      <c r="I46" s="29">
+        <v>18.408000000000001</v>
+      </c>
+      <c r="J46" s="29">
         <v>17.594999999999999</v>
       </c>
     </row>
-    <row r="47" spans="2:10" s="40" customFormat="1">
-      <c r="B47" s="40" t="s">
+    <row r="47" spans="2:10" s="28" customFormat="1">
+      <c r="B47" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="J47" s="45">
+      <c r="H47" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="2:10" s="40" customFormat="1">
-      <c r="B48" s="40" t="s">
+      <c r="I47" s="33">
+        <v>1</v>
+      </c>
+      <c r="J47" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" s="28" customFormat="1">
+      <c r="B48" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="J48" s="45">
+      <c r="H48" s="33">
+        <v>1.542</v>
+      </c>
+      <c r="I48" s="33">
+        <v>0.78</v>
+      </c>
+      <c r="J48" s="33">
         <v>3.476</v>
       </c>
     </row>
@@ -2331,7 +2673,13 @@
       <c r="B49" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J49" s="41">
+      <c r="H49" s="29">
+        <v>2.871</v>
+      </c>
+      <c r="I49" s="29">
+        <v>2.9039999999999999</v>
+      </c>
+      <c r="J49" s="29">
         <v>3.484</v>
       </c>
     </row>
@@ -2339,7 +2687,13 @@
       <c r="B50" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="J50" s="41">
+      <c r="H50" s="29">
+        <v>19.323</v>
+      </c>
+      <c r="I50" s="29">
+        <v>14.587999999999999</v>
+      </c>
+      <c r="J50" s="29">
         <v>18.908999999999999</v>
       </c>
     </row>
@@ -2347,7 +2701,13 @@
       <c r="B51" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J51" s="41">
+      <c r="H51" s="29">
+        <v>13.929</v>
+      </c>
+      <c r="I51" s="29">
+        <v>15.8223</v>
+      </c>
+      <c r="J51" s="29">
         <v>17.373000000000001</v>
       </c>
     </row>
@@ -2355,7 +2715,13 @@
       <c r="B52" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="J52" s="41">
+      <c r="H52" s="29">
+        <v>1.3089999999999999</v>
+      </c>
+      <c r="I52" s="29">
+        <v>1.829</v>
+      </c>
+      <c r="J52" s="29">
         <v>1.786</v>
       </c>
     </row>
@@ -2364,43 +2730,49 @@
         <v>105</v>
       </c>
       <c r="C53" s="3">
-        <f t="shared" ref="C53:I53" si="6">SUM(C46:C52)</f>
+        <f t="shared" ref="C53:I53" si="22">SUM(C46:C52)</f>
         <v>0</v>
       </c>
       <c r="D53" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="E53" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="F53" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="G53" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H53" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I53" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J53" s="41">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="H53" s="29">
+        <f t="shared" si="22"/>
+        <v>53.878999999999998</v>
+      </c>
+      <c r="I53" s="29">
+        <f t="shared" si="22"/>
+        <v>55.331299999999999</v>
+      </c>
+      <c r="J53" s="29">
         <f>SUM(J46:J52)</f>
         <v>63.623000000000005</v>
       </c>
     </row>
-    <row r="54" spans="2:10" s="40" customFormat="1">
-      <c r="B54" s="40" t="s">
+    <row r="54" spans="2:10" s="28" customFormat="1">
+      <c r="B54" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="J54" s="45">
+      <c r="H54" s="33">
+        <v>74.745000000000005</v>
+      </c>
+      <c r="I54" s="33">
+        <v>84.625</v>
+      </c>
+      <c r="J54" s="33">
         <v>89.512</v>
       </c>
     </row>
@@ -2408,7 +2780,13 @@
       <c r="B55" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J55" s="41">
+      <c r="H55" s="29">
+        <v>10.372999999999999</v>
+      </c>
+      <c r="I55" s="29">
+        <v>9.5030000000000001</v>
+      </c>
+      <c r="J55" s="29">
         <v>11.379</v>
       </c>
     </row>
@@ -2416,7 +2794,13 @@
       <c r="B56" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="J56" s="41">
+      <c r="H56" s="29">
+        <v>20.335999999999999</v>
+      </c>
+      <c r="I56" s="29">
+        <v>3.9430000000000001</v>
+      </c>
+      <c r="J56" s="29">
         <v>3.093</v>
       </c>
     </row>
@@ -2424,7 +2808,13 @@
       <c r="B57" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="J57" s="41">
+      <c r="H57" s="29">
+        <v>5.6680000000000001</v>
+      </c>
+      <c r="I57" s="29">
+        <v>3.7719999999999998</v>
+      </c>
+      <c r="J57" s="29">
         <v>1.637</v>
       </c>
     </row>
@@ -2432,7 +2822,13 @@
       <c r="B58" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J58" s="41">
+      <c r="H58" s="29">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="I58" s="29">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="J58" s="29">
         <v>0.32500000000000001</v>
       </c>
     </row>
@@ -2441,46 +2837,53 @@
         <v>111</v>
       </c>
       <c r="C59" s="3">
-        <f t="shared" ref="C59:I59" si="7">SUM(C53:C58)</f>
+        <f t="shared" ref="C59:I59" si="23">SUM(C53:C58)</f>
         <v>0</v>
       </c>
       <c r="D59" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="E59" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="F59" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="G59" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H59" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I59" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J59" s="41">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="H59" s="29">
+        <f t="shared" si="23"/>
+        <v>165.60999999999999</v>
+      </c>
+      <c r="I59" s="29">
+        <f t="shared" si="23"/>
+        <v>157.49929999999998</v>
+      </c>
+      <c r="J59" s="29">
         <f>SUM(J53:J58)</f>
         <v>169.56899999999996</v>
       </c>
     </row>
     <row r="60" spans="2:10">
-      <c r="J60" s="41"/>
+      <c r="H60" s="29"/>
+      <c r="J60" s="29"/>
     </row>
     <row r="61" spans="2:10">
       <c r="B61" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="J61" s="41">
+      <c r="H61" s="29">
+        <v>94.212000000000003</v>
+      </c>
+      <c r="I61" s="29">
+        <v>21.097999999999999</v>
+      </c>
+      <c r="J61" s="29">
         <v>14.803000000000001</v>
       </c>
     </row>
@@ -2488,7 +2891,15 @@
       <c r="B62" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="J62" s="41">
+      <c r="H62" s="29">
+        <f>H61+H59</f>
+        <v>259.822</v>
+      </c>
+      <c r="I62" s="29">
+        <f>I61+I59</f>
+        <v>178.59729999999996</v>
+      </c>
+      <c r="J62" s="29">
         <f>J61+J59</f>
         <v>184.37199999999996</v>
       </c>
@@ -2497,7 +2908,15 @@
       <c r="B64" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J64" s="41">
+      <c r="H64" s="29">
+        <f t="shared" ref="H64:I64" si="24">H44-H59</f>
+        <v>94.212000000000018</v>
+      </c>
+      <c r="I64" s="29">
+        <f>I44-I59</f>
+        <v>21.078700000000026</v>
+      </c>
+      <c r="J64" s="29">
         <f>J44-J59</f>
         <v>14.803000000000054</v>
       </c>
@@ -2506,6 +2925,14 @@
       <c r="B65" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="H65" s="3">
+        <f t="shared" ref="H65" si="25">H64/H19</f>
+        <v>1.5028025851739273</v>
+      </c>
+      <c r="I65" s="3">
+        <f>I64/I19</f>
+        <v>0.33462262003636223</v>
+      </c>
       <c r="J65" s="3">
         <f>J64/J19</f>
         <v>0.23326311172928102</v>
@@ -2515,7 +2942,15 @@
       <c r="B67" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J67" s="41">
+      <c r="H67" s="29">
+        <f t="shared" ref="H67:I67" si="26">H32</f>
+        <v>5.9379999999999997</v>
+      </c>
+      <c r="I67" s="29">
+        <f t="shared" ref="I67:J67" si="27">I32</f>
+        <v>10.879</v>
+      </c>
+      <c r="J67" s="29">
         <f>J32</f>
         <v>7.0309999999999997</v>
       </c>
@@ -2524,7 +2959,15 @@
       <c r="B68" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J68" s="41">
+      <c r="H68" s="29">
+        <f t="shared" ref="H68:I68" si="28">H47+H48+H54</f>
+        <v>77.287000000000006</v>
+      </c>
+      <c r="I68" s="29">
+        <f t="shared" ref="I68:J68" si="29">I47+I48+I54</f>
+        <v>86.405000000000001</v>
+      </c>
+      <c r="J68" s="29">
         <f>J47+J48+J54</f>
         <v>93.988</v>
       </c>
@@ -2533,7 +2976,15 @@
       <c r="B69" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J69" s="41">
+      <c r="H69" s="29">
+        <f t="shared" ref="H69" si="30">H67-H68</f>
+        <v>-71.349000000000004</v>
+      </c>
+      <c r="I69" s="29">
+        <f t="shared" ref="I69" si="31">I67-I68</f>
+        <v>-75.525999999999996</v>
+      </c>
+      <c r="J69" s="29">
         <f>J67-J68</f>
         <v>-86.956999999999994</v>
       </c>
@@ -2542,6 +2993,12 @@
       <c r="B71" s="3" t="s">
         <v>116</v>
       </c>
+      <c r="H71" s="3">
+        <v>8.48</v>
+      </c>
+      <c r="I71" s="3">
+        <v>3.04</v>
+      </c>
       <c r="J71" s="3">
         <v>2.38</v>
       </c>
@@ -2550,7 +3007,15 @@
       <c r="B72" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J72" s="41">
+      <c r="H72" s="29">
+        <f t="shared" ref="H72" si="32">H71*H19</f>
+        <v>531.61856912000007</v>
+      </c>
+      <c r="I72" s="29">
+        <f t="shared" ref="I72" si="33">I71*I19</f>
+        <v>191.49706016000002</v>
+      </c>
+      <c r="J72" s="29">
         <f>J71*J19</f>
         <v>151.03605425999999</v>
       </c>
@@ -2559,7 +3024,15 @@
       <c r="B73" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J73" s="41">
+      <c r="H73" s="29">
+        <f t="shared" ref="H73" si="34">H72-H69</f>
+        <v>602.96756912000012</v>
+      </c>
+      <c r="I73" s="29">
+        <f t="shared" ref="I73" si="35">I72-I69</f>
+        <v>267.02306016</v>
+      </c>
+      <c r="J73" s="29">
         <f>J72-J69</f>
         <v>237.99305425999998</v>
       </c>
@@ -2568,13 +3041,21 @@
       <c r="B75" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J75" s="50">
+      <c r="H75" s="36">
+        <f>H71/H65</f>
+        <v>5.6427903995244764</v>
+      </c>
+      <c r="I75" s="36">
+        <f>I71/I65</f>
+        <v>9.0848610284315328</v>
+      </c>
+      <c r="J75" s="36">
         <f>J71/J65</f>
         <v>10.203070611362524</v>
       </c>
     </row>
     <row r="79" spans="2:10">
-      <c r="B79" s="47" t="s">
+      <c r="B79" s="35" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2603,8 +3084,8 @@
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="2:2" s="40" customFormat="1">
-      <c r="B87" s="40" t="s">
+    <row r="87" spans="2:2" s="28" customFormat="1">
+      <c r="B87" s="28" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2613,16 +3094,19 @@
         <v>124</v>
       </c>
     </row>
-    <row r="90" spans="2:2" s="40" customFormat="1">
-      <c r="B90" s="40" t="s">
+    <row r="90" spans="2:2" s="28" customFormat="1">
+      <c r="B90" s="28" t="s">
         <v>125</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J1" r:id="rId1" location="ieb75bb50d25b43988f02e27af34ce5ea_19" xr:uid="{F3BAE21F-8075-4AD3-AE46-BE3F41688B15}"/>
+    <hyperlink ref="I1" r:id="rId2" xr:uid="{F513A548-D519-49B7-AE7F-0E259055CDF8}"/>
+    <hyperlink ref="H1" r:id="rId3" xr:uid="{36B2AE0E-4BDC-4E69-B27A-97F8E2FAB951}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q422 & FY22 projection
</commit_message>
<xml_diff>
--- a/$RDW.xlsx
+++ b/$RDW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DC895E-26B0-4DE1-9BC9-90CB06EE6630}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D60F6A-FE30-42BF-8452-F5BD95294F42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{DCD3578D-FA8F-4742-9003-583D815C10F0}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="130">
   <si>
     <t>$RDW</t>
   </si>
@@ -649,7 +649,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -793,6 +793,9 @@
     <xf numFmtId="9" fontId="13" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -895,7 +898,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6848475" y="0"/>
-          <a:ext cx="0" cy="16906875"/>
+          <a:ext cx="0" cy="17716500"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1271,7 +1274,7 @@
   <dimension ref="A2:N38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C33" sqref="C33:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1736,29 +1739,41 @@
       <c r="B34" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="37"/>
-      <c r="D34" s="38"/>
+      <c r="C34" s="47">
+        <f>C8/SUM('Financial Model'!$G$4:$J$4)</f>
+        <v>1.7051097255930614</v>
+      </c>
+      <c r="D34" s="48"/>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="38"/>
+      <c r="C35" s="47">
+        <f>C12/SUM('Financial Model'!$G$4:$J$4)</f>
+        <v>2.2929787620251627</v>
+      </c>
+      <c r="D35" s="48"/>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="37"/>
-      <c r="D36" s="38"/>
+      <c r="C36" s="47">
+        <f>C6/SUM('Financial Model'!G18:J18)</f>
+        <v>-2.0081225834964362</v>
+      </c>
+      <c r="D36" s="48"/>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="37"/>
-      <c r="D37" s="38"/>
+      <c r="C37" s="47">
+        <f>C12/SUM('Financial Model'!G17:J17)</f>
+        <v>-2.8633488569402465</v>
+      </c>
+      <c r="D37" s="48"/>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="12" t="s">
@@ -1810,7 +1825,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R21" sqref="R21"/>
+      <selection pane="bottomRight" activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2018,11 +2033,17 @@
       <c r="J5" s="29">
         <v>29.3</v>
       </c>
-      <c r="K5" s="65"/>
+      <c r="K5" s="65">
+        <f>K4*(1-K24)</f>
+        <v>35.759039999999999</v>
+      </c>
       <c r="Q5" s="29">
         <v>108.224</v>
       </c>
-      <c r="R5" s="56"/>
+      <c r="R5" s="56">
+        <f>SUM(H5:K5)</f>
+        <v>122.50104</v>
+      </c>
     </row>
     <row r="6" spans="1:31" s="33" customFormat="1">
       <c r="B6" s="33" t="s">
@@ -2060,12 +2081,18 @@
         <f>J4-J5</f>
         <v>7.9490000000000016</v>
       </c>
-      <c r="K6" s="64"/>
+      <c r="K6" s="64">
+        <f>K4-K5</f>
+        <v>8.9397599999999997</v>
+      </c>
       <c r="Q6" s="33">
         <f>Q4-Q5</f>
         <v>29.376999999999995</v>
       </c>
-      <c r="R6" s="55"/>
+      <c r="R6" s="55">
+        <f>R4-R5</f>
+        <v>29.041759999999996</v>
+      </c>
     </row>
     <row r="7" spans="1:31" s="29" customFormat="1">
       <c r="B7" s="29" t="s">
@@ -2093,11 +2120,17 @@
       <c r="J7" s="29">
         <v>15.311999999999999</v>
       </c>
-      <c r="K7" s="65"/>
+      <c r="K7" s="65">
+        <f>K4*0.56</f>
+        <v>25.031328000000002</v>
+      </c>
       <c r="Q7" s="29">
         <v>78.694999999999993</v>
       </c>
-      <c r="R7" s="56"/>
+      <c r="R7" s="56">
+        <f>SUM(H7:K7)</f>
+        <v>78.856328000000005</v>
+      </c>
     </row>
     <row r="8" spans="1:31" s="29" customFormat="1">
       <c r="B8" s="29" t="s">
@@ -2125,11 +2158,17 @@
       <c r="J8" s="29">
         <v>0</v>
       </c>
-      <c r="K8" s="65"/>
+      <c r="K8" s="65">
+        <f>J8</f>
+        <v>0</v>
+      </c>
       <c r="Q8" s="29">
         <v>11.337</v>
       </c>
-      <c r="R8" s="56"/>
+      <c r="R8" s="56">
+        <f t="shared" ref="R8:R11" si="2">SUM(H8:K8)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:31" s="29" customFormat="1">
       <c r="B9" s="29" t="s">
@@ -2157,11 +2196,17 @@
       <c r="J9" s="29">
         <v>1.819</v>
       </c>
-      <c r="K9" s="65"/>
+      <c r="K9" s="65">
+        <f>AVERAGE(G9:J9)</f>
+        <v>0.84550000000000014</v>
+      </c>
       <c r="Q9" s="29">
         <v>5.016</v>
       </c>
-      <c r="R9" s="56"/>
+      <c r="R9" s="56">
+        <f t="shared" si="2"/>
+        <v>2.7585000000000002</v>
+      </c>
     </row>
     <row r="10" spans="1:31" s="29" customFormat="1">
       <c r="B10" s="29" t="s">
@@ -2189,11 +2234,15 @@
       <c r="J10" s="29">
         <v>0</v>
       </c>
-      <c r="K10" s="65"/>
+      <c r="K10" s="65">
+        <v>0</v>
+      </c>
       <c r="Q10" s="29">
         <v>0</v>
       </c>
-      <c r="R10" s="56"/>
+      <c r="R10" s="56">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:31" s="29" customFormat="1">
       <c r="B11" s="29" t="s">
@@ -2221,54 +2270,66 @@
       <c r="J11" s="29">
         <v>1.133</v>
       </c>
-      <c r="K11" s="65"/>
+      <c r="K11" s="65">
+        <f>K4*K29</f>
+        <v>1.787952</v>
+      </c>
       <c r="Q11" s="29">
         <v>4.516</v>
       </c>
-      <c r="R11" s="56"/>
+      <c r="R11" s="56">
+        <f t="shared" si="2"/>
+        <v>6.3529519999999993</v>
+      </c>
     </row>
     <row r="12" spans="1:31" s="33" customFormat="1">
       <c r="B12" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="29">
-        <f t="shared" ref="C12:I12" si="2">C6-C7-C8-C9-C10-C11</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="29">
-        <f t="shared" si="2"/>
+      <c r="C12" s="33">
+        <f t="shared" ref="C12:I12" si="3">C6-C7-C8-C9-C10-C11</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <f t="shared" si="3"/>
         <v>-7.1920000000000002</v>
       </c>
-      <c r="E12" s="29">
-        <f t="shared" si="2"/>
+      <c r="E12" s="33">
+        <f t="shared" si="3"/>
         <v>-15.602999999999998</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="33">
         <f>F6-F7-F8-F9-F10-F11</f>
         <v>-31.050999999999998</v>
       </c>
-      <c r="G12" s="29">
-        <f t="shared" si="2"/>
+      <c r="G12" s="33">
+        <f t="shared" si="3"/>
         <v>-16.341000000000012</v>
       </c>
-      <c r="H12" s="29">
-        <f t="shared" si="2"/>
+      <c r="H12" s="33">
+        <f t="shared" si="3"/>
         <v>-17.550000000000004</v>
       </c>
-      <c r="I12" s="29">
-        <f t="shared" si="2"/>
+      <c r="I12" s="33">
+        <f t="shared" si="3"/>
         <v>-92.798000000000002</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J12" s="33">
         <f>J6-J7-J8-J9-J10-J11</f>
         <v>-10.314999999999998</v>
       </c>
-      <c r="K12" s="64"/>
-      <c r="Q12" s="29">
+      <c r="K12" s="64">
+        <f>K6-K7-K8-K9-K10-K11</f>
+        <v>-18.725020000000004</v>
+      </c>
+      <c r="Q12" s="33">
         <f>Q6-Q7-Q8-Q9-Q10-Q11</f>
         <v>-70.187000000000012</v>
       </c>
-      <c r="R12" s="55"/>
+      <c r="R12" s="64">
+        <f>R6-R7-R8-R9-R10-R11</f>
+        <v>-58.926020000000008</v>
+      </c>
     </row>
     <row r="13" spans="1:31" s="29" customFormat="1">
       <c r="B13" s="29" t="s">
@@ -2284,7 +2345,7 @@
         <v>1.74</v>
       </c>
       <c r="G13" s="29">
-        <f t="shared" ref="G13:G14" si="3">Q13-SUM(D13:F13)</f>
+        <f t="shared" ref="G13:G14" si="4">Q13-SUM(D13:F13)</f>
         <v>1.5250000000000004</v>
       </c>
       <c r="H13" s="29">
@@ -2296,11 +2357,17 @@
       <c r="J13" s="29">
         <v>2.4009999999999998</v>
       </c>
-      <c r="K13" s="65"/>
+      <c r="K13" s="65">
+        <f>AVERAGE(G13:J13)</f>
+        <v>1.762</v>
+      </c>
       <c r="Q13" s="29">
         <v>6.4560000000000004</v>
       </c>
-      <c r="R13" s="56"/>
+      <c r="R13" s="56">
+        <f t="shared" ref="R13:R14" si="5">SUM(H13:K13)</f>
+        <v>7.2850000000000001</v>
+      </c>
     </row>
     <row r="14" spans="1:31" s="29" customFormat="1">
       <c r="B14" s="29" t="s">
@@ -2316,7 +2383,7 @@
         <v>-2.9569999999999999</v>
       </c>
       <c r="G14" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.85700000000000021</v>
       </c>
       <c r="H14" s="29">
@@ -2328,26 +2395,32 @@
       <c r="J14" s="29">
         <v>-0.158</v>
       </c>
-      <c r="K14" s="65"/>
+      <c r="K14" s="65">
+        <f>AVERAGE(G14:J14)</f>
+        <v>-3.8374999999999999</v>
+      </c>
       <c r="Q14" s="29">
         <v>-3.8370000000000002</v>
       </c>
-      <c r="R14" s="56"/>
+      <c r="R14" s="56">
+        <f t="shared" si="5"/>
+        <v>-18.330500000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:31" s="29" customFormat="1">
       <c r="B15" s="29" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="29">
-        <f t="shared" ref="C15:I15" si="4">C12-C13-C14</f>
+        <f t="shared" ref="C15:I15" si="6">C12-C13-C14</f>
         <v>0</v>
       </c>
       <c r="D15" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-8.6999999999999993</v>
       </c>
       <c r="E15" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-17.262999999999998</v>
       </c>
       <c r="F15" s="29">
@@ -2355,27 +2428,33 @@
         <v>-29.833999999999996</v>
       </c>
       <c r="G15" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-17.009000000000015</v>
       </c>
       <c r="H15" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-20.182000000000002</v>
       </c>
       <c r="I15" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-78.953000000000003</v>
       </c>
       <c r="J15" s="29">
         <f>J12-J13-J14</f>
         <v>-12.557999999999998</v>
       </c>
-      <c r="K15" s="65"/>
+      <c r="K15" s="65">
+        <f>K12-K13-K14</f>
+        <v>-16.649520000000006</v>
+      </c>
       <c r="Q15" s="29">
         <f>Q12-Q13-Q14</f>
         <v>-72.806000000000012</v>
       </c>
-      <c r="R15" s="56"/>
+      <c r="R15" s="65">
+        <f>R12-R13-R14</f>
+        <v>-47.880520000000004</v>
+      </c>
     </row>
     <row r="16" spans="1:31" s="29" customFormat="1">
       <c r="B16" s="29" t="s">
@@ -2403,26 +2482,32 @@
       <c r="J16" s="29">
         <v>-2.1349999999999998</v>
       </c>
-      <c r="K16" s="65"/>
+      <c r="K16" s="65">
+        <f>K15*K27</f>
+        <v>-2.4974280000000006</v>
+      </c>
       <c r="Q16" s="29">
         <v>-11.269</v>
       </c>
-      <c r="R16" s="56"/>
+      <c r="R16" s="56">
+        <f>SUM(H16:K16)</f>
+        <v>-9.4464280000000009</v>
+      </c>
     </row>
     <row r="17" spans="2:18" s="33" customFormat="1">
       <c r="B17" s="33" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="33">
-        <f t="shared" ref="C17:I17" si="5">C15-C16</f>
+        <f t="shared" ref="C17:I17" si="7">C15-C16</f>
         <v>0</v>
       </c>
       <c r="D17" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-7.6739999999999995</v>
       </c>
       <c r="E17" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-15.900999999999998</v>
       </c>
       <c r="F17" s="33">
@@ -2430,27 +2515,33 @@
         <v>-24.251999999999995</v>
       </c>
       <c r="G17" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-13.710000000000015</v>
       </c>
       <c r="H17" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-17.293000000000003</v>
       </c>
       <c r="I17" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-77.028000000000006</v>
       </c>
       <c r="J17" s="33">
         <f>J15-J16</f>
         <v>-10.422999999999998</v>
       </c>
-      <c r="K17" s="64"/>
+      <c r="K17" s="64">
+        <f>K15-K16</f>
+        <v>-14.152092000000005</v>
+      </c>
       <c r="Q17" s="33">
         <f>Q15-Q16</f>
         <v>-61.537000000000013</v>
       </c>
-      <c r="R17" s="55"/>
+      <c r="R17" s="64">
+        <f>R15-R16</f>
+        <v>-38.434092000000007</v>
+      </c>
     </row>
     <row r="18" spans="2:18" s="31" customFormat="1">
       <c r="B18" s="31" t="s">
@@ -2484,12 +2575,18 @@
         <f>J17/J19</f>
         <v>-0.16424382986923508</v>
       </c>
-      <c r="K18" s="66"/>
+      <c r="K18" s="66">
+        <f>K17/K19</f>
+        <v>-0.22300621613180119</v>
+      </c>
       <c r="Q18" s="31">
         <f>Q17/Q19</f>
         <v>-1.3649850815872329</v>
       </c>
-      <c r="R18" s="57"/>
+      <c r="R18" s="57">
+        <f>R17/R19</f>
+        <v>-0.60563776912851686</v>
+      </c>
     </row>
     <row r="19" spans="2:18" s="29" customFormat="1">
       <c r="B19" s="29" t="s">
@@ -2517,11 +2614,17 @@
       <c r="J19" s="29">
         <v>63.460526999999999</v>
       </c>
-      <c r="K19" s="65"/>
+      <c r="K19" s="65">
+        <f>J19</f>
+        <v>63.460526999999999</v>
+      </c>
       <c r="Q19" s="29">
         <v>45.082543999999999</v>
       </c>
-      <c r="R19" s="56"/>
+      <c r="R19" s="56">
+        <f>K19</f>
+        <v>63.460526999999999</v>
+      </c>
     </row>
     <row r="21" spans="2:18" s="28" customFormat="1">
       <c r="B21" s="28" t="s">
@@ -2559,11 +2662,11 @@
         <v>1.6548463356973908E-2</v>
       </c>
       <c r="G22" s="30">
-        <f t="shared" ref="G22:H22" si="6">G4/F4-1</f>
+        <f t="shared" ref="G22:H22" si="8">G4/F4-1</f>
         <v>0.25688494492044023</v>
       </c>
       <c r="H22" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.19982958003651841</v>
       </c>
       <c r="I22" s="30">
@@ -2580,17 +2683,20 @@
       <c r="Q22" s="51" t="s">
         <v>127</v>
       </c>
+      <c r="R22" s="71" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D24" s="30">
-        <f t="shared" ref="D24:E24" si="7">D6/D4</f>
+        <f t="shared" ref="D24:E24" si="9">D6/D4</f>
         <v>0.23588239005615497</v>
       </c>
       <c r="E24" s="30">
-        <f t="shared" ref="E24:F24" si="8">E6/E4</f>
+        <f t="shared" ref="E24:F24" si="10">E6/E4</f>
         <v>0.26794823939280837</v>
       </c>
       <c r="F24" s="30">
@@ -2598,36 +2704,42 @@
         <v>0.18035495716034267</v>
       </c>
       <c r="G24" s="30">
-        <f t="shared" ref="G24" si="9">G6/G4</f>
+        <f t="shared" ref="G24" si="11">G6/G4</f>
         <v>0.17996348143639643</v>
       </c>
       <c r="H24" s="30">
-        <f t="shared" ref="H24:I24" si="10">H6/H4</f>
+        <f t="shared" ref="H24:I24" si="12">H6/H4</f>
         <v>0.15733106155109977</v>
       </c>
       <c r="I24" s="30">
-        <f t="shared" ref="I24:J24" si="11">I6/I4</f>
+        <f t="shared" ref="I24:J24" si="13">I6/I4</f>
         <v>0.19010019603572215</v>
       </c>
       <c r="J24" s="30">
         <f>J6/J4</f>
         <v>0.21340170205911571</v>
       </c>
+      <c r="K24" s="68">
+        <v>0.2</v>
+      </c>
       <c r="Q24" s="30">
         <f>Q6/Q4</f>
         <v>0.21349408797901176</v>
       </c>
+      <c r="R24" s="68">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D25" s="30">
-        <f t="shared" ref="D25:E25" si="12">D12/D4</f>
+        <f t="shared" ref="D25:E25" si="14">D12/D4</f>
         <v>-0.22689128651649948</v>
       </c>
       <c r="E25" s="30">
-        <f t="shared" ref="E25:F25" si="13">E12/E4</f>
+        <f t="shared" ref="E25:F25" si="15">E12/E4</f>
         <v>-0.48534901082493459</v>
       </c>
       <c r="F25" s="30">
@@ -2635,36 +2747,44 @@
         <v>-0.95015299877600978</v>
       </c>
       <c r="G25" s="30">
-        <f t="shared" ref="G25" si="14">G12/G4</f>
+        <f t="shared" ref="G25" si="16">G12/G4</f>
         <v>-0.39783323189287928</v>
       </c>
       <c r="H25" s="30">
-        <f t="shared" ref="H25:I25" si="15">H12/H4</f>
+        <f t="shared" ref="H25:I25" si="17">H12/H4</f>
         <v>-0.53397024370949597</v>
       </c>
       <c r="I25" s="30">
-        <f t="shared" ref="I25:J25" si="16">I12/I4</f>
+        <f t="shared" ref="I25:J25" si="18">I12/I4</f>
         <v>-2.5266281855804835</v>
       </c>
       <c r="J25" s="30">
         <f>J12/J4</f>
         <v>-0.27692018577679928</v>
       </c>
+      <c r="K25" s="68">
+        <f>K12/K4</f>
+        <v>-0.41891549661288457</v>
+      </c>
       <c r="Q25" s="30">
         <f>Q12/Q4</f>
         <v>-0.51007623491108356</v>
       </c>
+      <c r="R25" s="68">
+        <f>R12/R4</f>
+        <v>-0.38884077633513442</v>
+      </c>
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D26" s="30">
-        <f t="shared" ref="D26:E26" si="17">D17/D4</f>
+        <f t="shared" ref="D26:E26" si="19">D17/D4</f>
         <v>-0.24209729320461856</v>
       </c>
       <c r="E26" s="30">
-        <f t="shared" ref="E26:F26" si="18">E17/E4</f>
+        <f t="shared" ref="E26:F26" si="20">E17/E4</f>
         <v>-0.49461863879557039</v>
       </c>
       <c r="F26" s="30">
@@ -2672,36 +2792,44 @@
         <v>-0.7421052631578946</v>
       </c>
       <c r="G26" s="30">
-        <f t="shared" ref="G26" si="19">G17/G4</f>
+        <f t="shared" ref="G26" si="21">G17/G4</f>
         <v>-0.33377967133292802</v>
       </c>
       <c r="H26" s="30">
-        <f t="shared" ref="H26:I26" si="20">H17/H4</f>
+        <f t="shared" ref="H26:I26" si="22">H17/H4</f>
         <v>-0.52615085039705489</v>
       </c>
       <c r="I26" s="30">
-        <f t="shared" ref="I26:J26" si="21">I17/I4</f>
+        <f t="shared" ref="I26:J26" si="23">I17/I4</f>
         <v>-2.0972554998910913</v>
       </c>
       <c r="J26" s="30">
         <f>J17/J4</f>
         <v>-0.27981959247228105</v>
       </c>
+      <c r="K26" s="68">
+        <f>K17/K4</f>
+        <v>-0.3166101103385327</v>
+      </c>
       <c r="Q26" s="30">
         <f>Q17/Q4</f>
         <v>-0.44721331967064204</v>
       </c>
+      <c r="R26" s="68">
+        <f>R17/R4</f>
+        <v>-0.25361872685472359</v>
+      </c>
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D27" s="30">
-        <f t="shared" ref="D27:E27" si="22">D16/D15</f>
+        <f t="shared" ref="D27:E27" si="24">D16/D15</f>
         <v>0.11793103448275863</v>
       </c>
       <c r="E27" s="30">
-        <f t="shared" ref="E27:F27" si="23">E16/E15</f>
+        <f t="shared" ref="E27:F27" si="25">E16/E15</f>
         <v>7.889706308289407E-2</v>
       </c>
       <c r="F27" s="30">
@@ -2709,64 +2837,75 @@
         <v>0.1871019642019173</v>
       </c>
       <c r="G27" s="30">
-        <f t="shared" ref="G27" si="24">G16/G15</f>
+        <f t="shared" ref="G27" si="26">G16/G15</f>
         <v>0.1939561408665999</v>
       </c>
       <c r="H27" s="30">
-        <f t="shared" ref="H27:I27" si="25">H16/H15</f>
+        <f t="shared" ref="H27:I27" si="27">H16/H15</f>
         <v>0.14314735903280149</v>
       </c>
       <c r="I27" s="30">
-        <f t="shared" ref="I27:J27" si="26">I16/I15</f>
+        <f t="shared" ref="I27:J27" si="28">I16/I15</f>
         <v>2.4381594112953275E-2</v>
       </c>
       <c r="J27" s="30">
         <f>J16/J15</f>
         <v>0.17001114827201785</v>
       </c>
+      <c r="K27" s="68">
+        <v>0.15</v>
+      </c>
       <c r="Q27" s="30">
         <f>Q16/Q15</f>
         <v>0.15478119935170176</v>
       </c>
+      <c r="R27" s="68">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="29" spans="2:18" s="30" customFormat="1">
       <c r="B29" s="30" t="s">
         <v>126</v>
       </c>
       <c r="D29" s="30">
-        <f t="shared" ref="D29:F29" si="27">D11/D4</f>
+        <f t="shared" ref="D29:F29" si="29">D11/D4</f>
         <v>3.142154079121711E-2</v>
       </c>
       <c r="E29" s="30">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>2.9799676496205046E-2</v>
       </c>
       <c r="F29" s="30">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>4.1952264381884943E-2</v>
       </c>
       <c r="G29" s="30">
-        <f t="shared" ref="G29" si="28">G11/G4</f>
+        <f t="shared" ref="G29" si="30">G11/G4</f>
         <v>2.8995739500912967E-2</v>
       </c>
       <c r="H29" s="30">
-        <f t="shared" ref="H29:J29" si="29">H11/H4</f>
+        <f t="shared" ref="H29:J29" si="31">H11/H4</f>
         <v>5.2453829068670708E-2</v>
       </c>
       <c r="I29" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>4.6504029623175777E-2</v>
       </c>
       <c r="J29" s="30">
         <f>J11/J4</f>
         <v>3.0416923944266958E-2</v>
       </c>
-      <c r="K29" s="68"/>
+      <c r="K29" s="68">
+        <v>0.04</v>
+      </c>
       <c r="Q29" s="30">
         <f>Q11/Q4</f>
         <v>3.2819528927842095E-2</v>
       </c>
-      <c r="R29" s="60"/>
+      <c r="R29" s="60">
+        <f>R11/R4</f>
+        <v>4.1921833303858708E-2</v>
+      </c>
     </row>
     <row r="32" spans="2:18">
       <c r="B32" s="35" t="s">
@@ -2834,7 +2973,7 @@
         <v>16.318999999999999</v>
       </c>
       <c r="Q35" s="29">
-        <f t="shared" ref="Q35:Q44" si="30">G35</f>
+        <f t="shared" ref="Q35:Q44" si="32">G35</f>
         <v>11.747999999999999</v>
       </c>
     </row>
@@ -2855,7 +2994,7 @@
         <v>2.0289999999999999</v>
       </c>
       <c r="Q36" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.68799999999999994</v>
       </c>
     </row>
@@ -2876,7 +3015,7 @@
         <v>0.68799999999999994</v>
       </c>
       <c r="Q37" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.68799999999999994</v>
       </c>
     </row>
@@ -2897,7 +3036,7 @@
         <v>3.0459999999999998</v>
       </c>
       <c r="Q38" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>2.819</v>
       </c>
     </row>
@@ -2918,7 +3057,7 @@
         <v>3.7250000000000001</v>
       </c>
       <c r="Q39" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>2.488</v>
       </c>
     </row>
@@ -2927,31 +3066,31 @@
         <v>92</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" ref="C40:I40" si="31">SUM(C33:C39)</f>
+        <f t="shared" ref="C40:I40" si="33">SUM(C33:C39)</f>
         <v>0</v>
       </c>
       <c r="D40" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="E40" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="F40" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="G40" s="29">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>55.216000000000001</v>
       </c>
       <c r="H40" s="29">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>43.469000000000008</v>
       </c>
       <c r="I40" s="29">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>45.442</v>
       </c>
       <c r="J40" s="29">
@@ -2959,7 +3098,7 @@
         <v>49.358999999999995</v>
       </c>
       <c r="Q40" s="29">
-        <f t="shared" ref="Q40" si="32">SUM(Q33:Q39)</f>
+        <f t="shared" ref="Q40" si="34">SUM(Q33:Q39)</f>
         <v>55.216000000000001</v>
       </c>
     </row>
@@ -2980,7 +3119,7 @@
         <v>6.6970000000000001</v>
       </c>
       <c r="Q41" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>19.384</v>
       </c>
     </row>
@@ -3001,7 +3140,7 @@
         <v>14.782999999999999</v>
       </c>
       <c r="Q42" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -3026,7 +3165,7 @@
         <v>112.917</v>
       </c>
       <c r="Q43" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>187.15600000000001</v>
       </c>
     </row>
@@ -3047,7 +3186,7 @@
         <v>0.61599999999999999</v>
       </c>
       <c r="Q44" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -3056,31 +3195,31 @@
         <v>97</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" ref="C45:I45" si="33">C40+SUM(C41:C44)</f>
+        <f t="shared" ref="C45:I45" si="35">C40+SUM(C41:C44)</f>
         <v>0</v>
       </c>
       <c r="D45" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="E45" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="F45" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="G45" s="29">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>261.75600000000003</v>
       </c>
       <c r="H45" s="29">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>259.822</v>
       </c>
       <c r="I45" s="29">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>178.578</v>
       </c>
       <c r="J45" s="29">
@@ -3088,7 +3227,7 @@
         <v>184.37200000000001</v>
       </c>
       <c r="Q45" s="29">
-        <f t="shared" ref="Q45" si="34">Q40+SUM(Q41:Q44)</f>
+        <f t="shared" ref="Q45" si="36">Q40+SUM(Q41:Q44)</f>
         <v>261.75600000000003</v>
       </c>
     </row>
@@ -3113,7 +3252,7 @@
         <v>17.594999999999999</v>
       </c>
       <c r="Q47" s="29">
-        <f t="shared" ref="Q47:Q53" si="35">G47</f>
+        <f t="shared" ref="Q47:Q53" si="37">G47</f>
         <v>13.131</v>
       </c>
     </row>
@@ -3135,7 +3274,7 @@
       </c>
       <c r="K48" s="70"/>
       <c r="Q48" s="33">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="R48" s="61"/>
@@ -3158,7 +3297,7 @@
       </c>
       <c r="K49" s="70"/>
       <c r="Q49" s="33">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>2.6840000000000002</v>
       </c>
       <c r="R49" s="61"/>
@@ -3180,7 +3319,7 @@
         <v>3.484</v>
       </c>
       <c r="Q50" s="29">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -3201,7 +3340,7 @@
         <v>18.908999999999999</v>
       </c>
       <c r="Q51" s="29">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>17.117999999999999</v>
       </c>
     </row>
@@ -3222,7 +3361,7 @@
         <v>17.373000000000001</v>
       </c>
       <c r="Q52" s="29">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>15.734</v>
       </c>
     </row>
@@ -3243,7 +3382,7 @@
         <v>1.786</v>
       </c>
       <c r="Q53" s="29">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>1.571</v>
       </c>
     </row>
@@ -3252,31 +3391,31 @@
         <v>105</v>
       </c>
       <c r="C54" s="3">
-        <f t="shared" ref="C54:I54" si="36">SUM(C47:C53)</f>
+        <f t="shared" ref="C54:I54" si="38">SUM(C47:C53)</f>
         <v>0</v>
       </c>
       <c r="D54" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="E54" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="F54" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G54" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>51.238</v>
       </c>
       <c r="H54" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>53.878999999999998</v>
       </c>
       <c r="I54" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>55.331299999999999</v>
       </c>
       <c r="J54" s="29">
@@ -3284,7 +3423,7 @@
         <v>63.623000000000005</v>
       </c>
       <c r="Q54" s="29">
-        <f t="shared" ref="Q54" si="37">SUM(Q47:Q53)</f>
+        <f t="shared" ref="Q54" si="39">SUM(Q47:Q53)</f>
         <v>51.238</v>
       </c>
     </row>
@@ -3328,7 +3467,7 @@
         <v>11.379</v>
       </c>
       <c r="Q56" s="29">
-        <f t="shared" ref="Q56:Q59" si="38">G56</f>
+        <f t="shared" ref="Q56:Q59" si="40">G56</f>
         <v>0</v>
       </c>
     </row>
@@ -3349,7 +3488,7 @@
         <v>3.093</v>
       </c>
       <c r="Q57" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>19.097999999999999</v>
       </c>
     </row>
@@ -3370,7 +3509,7 @@
         <v>1.637</v>
       </c>
       <c r="Q58" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>8.6010000000000009</v>
       </c>
     </row>
@@ -3391,7 +3530,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="Q59" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>0.73</v>
       </c>
     </row>
@@ -3400,31 +3539,31 @@
         <v>111</v>
       </c>
       <c r="C60" s="3">
-        <f t="shared" ref="C60:I60" si="39">SUM(C54:C59)</f>
+        <f t="shared" ref="C60:I60" si="41">SUM(C54:C59)</f>
         <v>0</v>
       </c>
       <c r="D60" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="E60" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="F60" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="G60" s="29">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>154.53399999999999</v>
       </c>
       <c r="H60" s="29">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>165.60999999999999</v>
       </c>
       <c r="I60" s="29">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>157.49929999999998</v>
       </c>
       <c r="J60" s="29">
@@ -3432,7 +3571,7 @@
         <v>169.56899999999996</v>
       </c>
       <c r="Q60" s="29">
-        <f t="shared" ref="Q60" si="40">SUM(Q54:Q59)</f>
+        <f t="shared" ref="Q60" si="42">SUM(Q54:Q59)</f>
         <v>154.53399999999999</v>
       </c>
     </row>
@@ -3466,7 +3605,7 @@
         <v>113</v>
       </c>
       <c r="G63" s="29">
-        <f t="shared" ref="G63" si="41">G62+G60</f>
+        <f t="shared" ref="G63" si="43">G62+G60</f>
         <v>261.75599999999997</v>
       </c>
       <c r="H63" s="29">
@@ -3491,11 +3630,11 @@
         <v>114</v>
       </c>
       <c r="G65" s="29">
-        <f t="shared" ref="G65:H65" si="42">G45-G60</f>
+        <f t="shared" ref="G65:H65" si="44">G45-G60</f>
         <v>107.22200000000004</v>
       </c>
       <c r="H65" s="29">
-        <f t="shared" ref="H65:I65" si="43">H45-H60</f>
+        <f t="shared" ref="H65:I65" si="45">H45-H60</f>
         <v>94.212000000000018</v>
       </c>
       <c r="I65" s="29">
@@ -3516,11 +3655,11 @@
         <v>115</v>
       </c>
       <c r="G66" s="3">
-        <f t="shared" ref="G66" si="44">G65/G19</f>
+        <f t="shared" ref="G66" si="46">G65/G19</f>
         <v>2.3783484800680288</v>
       </c>
       <c r="H66" s="3">
-        <f t="shared" ref="H66" si="45">H65/H19</f>
+        <f t="shared" ref="H66" si="47">H65/H19</f>
         <v>1.5028025851739273</v>
       </c>
       <c r="I66" s="3">
@@ -3541,15 +3680,15 @@
         <v>6</v>
       </c>
       <c r="G68" s="29">
-        <f t="shared" ref="G68:H68" si="46">G33</f>
+        <f t="shared" ref="G68:H68" si="48">G33</f>
         <v>20.523</v>
       </c>
       <c r="H68" s="29">
-        <f t="shared" ref="H68:I68" si="47">H33</f>
+        <f t="shared" ref="H68:I68" si="49">H33</f>
         <v>5.9379999999999997</v>
       </c>
       <c r="I68" s="29">
-        <f t="shared" ref="I68:J68" si="48">I33</f>
+        <f t="shared" ref="I68:J68" si="50">I33</f>
         <v>10.879</v>
       </c>
       <c r="J68" s="29">
@@ -3566,15 +3705,15 @@
         <v>7</v>
       </c>
       <c r="G69" s="29">
-        <f t="shared" ref="G69:H69" si="49">G48+G49+G55</f>
+        <f t="shared" ref="G69:H69" si="51">G48+G49+G55</f>
         <v>78.551000000000002</v>
       </c>
       <c r="H69" s="29">
-        <f t="shared" ref="H69:I69" si="50">H48+H49+H55</f>
+        <f t="shared" ref="H69:I69" si="52">H48+H49+H55</f>
         <v>77.287000000000006</v>
       </c>
       <c r="I69" s="29">
-        <f t="shared" ref="I69:J69" si="51">I48+I49+I55</f>
+        <f t="shared" ref="I69:J69" si="53">I48+I49+I55</f>
         <v>86.405000000000001</v>
       </c>
       <c r="J69" s="29">
@@ -3591,15 +3730,15 @@
         <v>8</v>
       </c>
       <c r="G70" s="29">
-        <f t="shared" ref="G70" si="52">G68-G69</f>
+        <f t="shared" ref="G70" si="54">G68-G69</f>
         <v>-58.028000000000006</v>
       </c>
       <c r="H70" s="29">
-        <f t="shared" ref="H70" si="53">H68-H69</f>
+        <f t="shared" ref="H70" si="55">H68-H69</f>
         <v>-71.349000000000004</v>
       </c>
       <c r="I70" s="29">
-        <f t="shared" ref="I70" si="54">I68-I69</f>
+        <f t="shared" ref="I70" si="56">I68-I69</f>
         <v>-75.525999999999996</v>
       </c>
       <c r="J70" s="29">
@@ -3637,15 +3776,15 @@
         <v>5</v>
       </c>
       <c r="G73" s="29">
-        <f t="shared" ref="G73" si="55">G72*G19</f>
+        <f t="shared" ref="G73" si="57">G72*G19</f>
         <v>304.30717199999998</v>
       </c>
       <c r="H73" s="29">
-        <f t="shared" ref="H73" si="56">H72*H19</f>
+        <f t="shared" ref="H73" si="58">H72*H19</f>
         <v>531.61856912000007</v>
       </c>
       <c r="I73" s="29">
-        <f t="shared" ref="I73" si="57">I72*I19</f>
+        <f t="shared" ref="I73" si="59">I72*I19</f>
         <v>191.49706016000002</v>
       </c>
       <c r="J73" s="29">
@@ -3653,7 +3792,7 @@
         <v>151.03605425999999</v>
       </c>
       <c r="Q73" s="29">
-        <f t="shared" ref="Q73" si="58">Q72*Q19</f>
+        <f t="shared" ref="Q73" si="60">Q72*Q19</f>
         <v>304.30717199999998</v>
       </c>
     </row>
@@ -3662,15 +3801,15 @@
         <v>9</v>
       </c>
       <c r="G74" s="29">
-        <f t="shared" ref="G74" si="59">G73-G70</f>
+        <f t="shared" ref="G74" si="61">G73-G70</f>
         <v>362.335172</v>
       </c>
       <c r="H74" s="29">
-        <f t="shared" ref="H74" si="60">H73-H70</f>
+        <f t="shared" ref="H74" si="62">H73-H70</f>
         <v>602.96756912000012</v>
       </c>
       <c r="I74" s="29">
-        <f t="shared" ref="I74" si="61">I73-I70</f>
+        <f t="shared" ref="I74" si="63">I73-I70</f>
         <v>267.02306016</v>
       </c>
       <c r="J74" s="29">
@@ -3678,7 +3817,7 @@
         <v>237.99305425999998</v>
       </c>
       <c r="Q74" s="29">
-        <f t="shared" ref="Q74" si="62">Q73-Q70</f>
+        <f t="shared" ref="Q74" si="64">Q73-Q70</f>
         <v>362.335172</v>
       </c>
     </row>
@@ -3691,7 +3830,7 @@
         <v>22</v>
       </c>
       <c r="G76" s="36">
-        <f t="shared" ref="G76:H76" si="63">G72/G66</f>
+        <f t="shared" ref="G76:H76" si="65">G72/G66</f>
         <v>2.8381038592826089</v>
       </c>
       <c r="H76" s="36">
@@ -3720,15 +3859,15 @@
         <v>23</v>
       </c>
       <c r="G77" s="36">
-        <f t="shared" ref="G77:J77" si="64">G73/SUM($G$4:$J$4)</f>
+        <f t="shared" ref="G77:J77" si="66">G73/SUM($G$4:$J$4)</f>
         <v>2.057255470899614</v>
       </c>
       <c r="H77" s="36">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>3.5939843368329973</v>
       </c>
       <c r="I77" s="36">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>1.2946075903704057</v>
       </c>
       <c r="J77" s="36">
@@ -3749,15 +3888,15 @@
         <v>24</v>
       </c>
       <c r="G78" s="36">
-        <f t="shared" ref="G78:J78" si="65">G74/SUM($G$4:$J$4)</f>
+        <f t="shared" ref="G78:J78" si="67">G74/SUM($G$4:$J$4)</f>
         <v>2.4495512544027478</v>
       </c>
       <c r="H78" s="36">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>4.076336164522476</v>
       </c>
       <c r="I78" s="36">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>1.8051978458480658</v>
       </c>
       <c r="J78" s="36">
@@ -3778,15 +3917,15 @@
         <v>25</v>
       </c>
       <c r="G79" s="36">
-        <f t="shared" ref="G79:I79" si="66">G72/SUM(D18:G18)</f>
+        <f t="shared" ref="G79:I79" si="68">G72/SUM(D18:G18)</f>
         <v>-4.5345346676411911</v>
       </c>
       <c r="H79" s="36">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>-5.442416520441185</v>
       </c>
       <c r="I79" s="36">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>-1.2916941654103256</v>
       </c>
       <c r="J79" s="36">
@@ -3807,15 +3946,15 @@
         <v>26</v>
       </c>
       <c r="G80" s="36">
-        <f t="shared" ref="G80:I80" si="67">G74/SUM(D17:G17)</f>
+        <f t="shared" ref="G80:I80" si="69">G74/SUM(D17:G17)</f>
         <v>-5.8880863870516915</v>
       </c>
       <c r="H80" s="36">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>-8.4738823025465191</v>
       </c>
       <c r="I80" s="36">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>-2.0185742700120195</v>
       </c>
       <c r="J80" s="36">
@@ -3945,11 +4084,11 @@
         <v>-1.014</v>
       </c>
       <c r="I94" s="29">
-        <f t="shared" ref="I94:J94" si="68">-I88+I89+I90</f>
+        <f t="shared" ref="I94:J94" si="70">-I88+I89+I90</f>
         <v>-1.0589999999999997</v>
       </c>
       <c r="J94" s="29">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>-1.3590000000000004</v>
       </c>
     </row>
@@ -3962,11 +4101,11 @@
         <v>-12.459999999999999</v>
       </c>
       <c r="I95" s="33">
-        <f t="shared" ref="I95" si="69">I86+I94</f>
+        <f t="shared" ref="I95" si="71">I86+I94</f>
         <v>-5.1969999999999992</v>
       </c>
       <c r="J95" s="33">
-        <f t="shared" ref="J95" si="70">J86+J94</f>
+        <f t="shared" ref="J95" si="72">J86+J94</f>
         <v>-12.604000000000001</v>
       </c>
       <c r="K95" s="70"/>
@@ -3981,7 +4120,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
   <ignoredErrors>
-    <ignoredError sqref="G6:G19 Q40:Q58" formula="1"/>
+    <ignoredError sqref="G6:G19 Q40:Q58 R6 R12:R18" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId5"/>
 </worksheet>

</xml_diff>